<commit_message>
atualiza url de fotos
</commit_message>
<xml_diff>
--- a/data-raw/lista_nao_senadores_preenchida.xlsx
+++ b/data-raw/lista_nao_senadores_preenchida.xlsx
@@ -123,9 +123,6 @@
     <t>https://pt.wikipedia.org/wiki/Ficheiro:2020-04-17_Solenidade_de_Posse_do_senhor_Nelson_Luiz_Sperle_Teich,_Ministro_de_Estado_da_Sa%C3%BAde_01_(cropped).jpg</t>
   </si>
   <si>
-    <t>https://pt.wikipedia.org/wiki/Ficheiro:CAS_-_Comiss%C3%A3o_de_Assuntos_Sociais_(35941643904)_(cropped).jpg</t>
-  </si>
-  <si>
     <t>http://www.toronadvogados.com.br/images/conteudo/toron.jpg</t>
   </si>
   <si>
@@ -211,6 +208,9 @@
   </si>
   <si>
     <t>url_foto</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/f/f6/CAS_-_Comiss%C3%A3o_de_Assuntos_Sociais_%2835941643904%29_%28cropped%29.jpg</t>
   </si>
 </sst>
 </file>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -598,7 +598,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -606,7 +606,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -614,7 +614,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -622,7 +622,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -630,7 +630,7 @@
         <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -638,7 +638,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -646,7 +646,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -654,7 +654,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -662,7 +662,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -670,7 +670,7 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -678,7 +678,7 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -686,7 +686,7 @@
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -694,7 +694,7 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -702,7 +702,7 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -710,7 +710,7 @@
         <v>29</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -718,7 +718,7 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -726,15 +726,15 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
         <v>61</v>
-      </c>
-      <c r="B19" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -742,7 +742,7 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -758,7 +758,7 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -766,7 +766,7 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -774,7 +774,7 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -782,7 +782,7 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -790,7 +790,7 @@
         <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -806,7 +806,7 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -814,7 +814,7 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -822,7 +822,7 @@
         <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -830,7 +830,7 @@
         <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -838,7 +838,7 @@
         <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -846,7 +846,7 @@
         <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualiza fotos com url quebrado
</commit_message>
<xml_diff>
--- a/data-raw/lista_nao_senadores_preenchida.xlsx
+++ b/data-raw/lista_nao_senadores_preenchida.xlsx
@@ -123,9 +123,6 @@
     <t>https://pt.wikipedia.org/wiki/Ficheiro:2020-04-17_Solenidade_de_Posse_do_senhor_Nelson_Luiz_Sperle_Teich,_Ministro_de_Estado_da_Sa%C3%BAde_01_(cropped).jpg</t>
   </si>
   <si>
-    <t>http://www.toronadvogados.com.br/images/conteudo/toron.jpg</t>
-  </si>
-  <si>
     <t>https://www12.senado.leg.br/noticias/materias/2019/07/10/senado-aprova-indicacao-de-antonio-barra-torres-para-diretor-da-anvisa/20190710_03311ls.jpg/@@images/image/imagem_materia</t>
   </si>
   <si>
@@ -211,6 +208,9 @@
   </si>
   <si>
     <t>https://upload.wikimedia.org/wikipedia/commons/f/f6/CAS_-_Comiss%C3%A3o_de_Assuntos_Sociais_%2835941643904%29_%28cropped%29.jpg</t>
+  </si>
+  <si>
+    <t>https://www.prerro.com.br/wp-content/uploads/2019/09/Alberto-Toron-bio2.png</t>
   </si>
 </sst>
 </file>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -590,15 +590,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s">
-        <v>34</v>
+      <c r="B2" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -606,7 +606,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -614,7 +614,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -622,7 +622,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -630,7 +630,7 @@
         <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -638,7 +638,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -646,7 +646,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -654,7 +654,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -662,7 +662,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -670,7 +670,7 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -678,7 +678,7 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -686,7 +686,7 @@
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -694,7 +694,7 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -702,7 +702,7 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -710,7 +710,7 @@
         <v>29</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -718,7 +718,7 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -726,15 +726,15 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" t="s">
         <v>60</v>
-      </c>
-      <c r="B19" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -742,7 +742,7 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -758,7 +758,7 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -766,7 +766,7 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -774,7 +774,7 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -782,7 +782,7 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -790,14 +790,14 @@
         <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>2</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -806,7 +806,7 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -814,7 +814,7 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -822,7 +822,7 @@
         <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -830,7 +830,7 @@
         <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -838,7 +838,7 @@
         <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -846,7 +846,7 @@
         <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -855,6 +855,8 @@
   </sortState>
   <hyperlinks>
     <hyperlink ref="B16" r:id="rId1"/>
+    <hyperlink ref="B27" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
correção de url de fotos
</commit_message>
<xml_diff>
--- a/data-raw/lista_nao_senadores_preenchida.xlsx
+++ b/data-raw/lista_nao_senadores_preenchida.xlsx
@@ -120,9 +120,6 @@
     <t>https://upload.wikimedia.org/wikipedia/commons/thumb/d/d4/Luiz_Henrique_Mandetta.jpg/210px-Luiz_Henrique_Mandetta.jpg</t>
   </si>
   <si>
-    <t>https://pt.wikipedia.org/wiki/Ficheiro:2020-04-17_Solenidade_de_Posse_do_senhor_Nelson_Luiz_Sperle_Teich,_Ministro_de_Estado_da_Sa%C3%BAde_01_(cropped).jpg</t>
-  </si>
-  <si>
     <t>https://www12.senado.leg.br/noticias/materias/2019/07/10/senado-aprova-indicacao-de-antonio-barra-torres-para-diretor-da-anvisa/20190710_03311ls.jpg/@@images/image/imagem_materia</t>
   </si>
   <si>
@@ -211,6 +208,9 @@
   </si>
   <si>
     <t>https://www.prerro.com.br/wp-content/uploads/2019/09/Alberto-Toron-bio2.png</t>
+  </si>
+  <si>
+    <t>https://static.ndmais.com.br/2020/05/49811303336_8f58832171_c.jpg</t>
   </si>
 </sst>
 </file>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -598,7 +598,7 @@
         <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -606,7 +606,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -614,7 +614,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -622,7 +622,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -630,7 +630,7 @@
         <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -638,7 +638,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -646,7 +646,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -654,7 +654,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -662,7 +662,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -670,7 +670,7 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -678,7 +678,7 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -686,7 +686,7 @@
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -694,7 +694,7 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -702,7 +702,7 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -710,7 +710,7 @@
         <v>29</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -718,7 +718,7 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -726,15 +726,15 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" t="s">
         <v>59</v>
-      </c>
-      <c r="B19" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -742,7 +742,7 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -758,7 +758,7 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -766,7 +766,7 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -774,7 +774,7 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -782,7 +782,7 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -790,7 +790,7 @@
         <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -798,7 +798,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -806,7 +806,7 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -814,7 +814,7 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -822,7 +822,7 @@
         <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -830,7 +830,7 @@
         <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -838,7 +838,7 @@
         <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -846,7 +846,7 @@
         <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -855,8 +855,7 @@
   </sortState>
   <hyperlinks>
     <hyperlink ref="B16" r:id="rId1"/>
-    <hyperlink ref="B27" r:id="rId2"/>
-    <hyperlink ref="B2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>